<commit_message>
update name teacher from database
</commit_message>
<xml_diff>
--- a/file_excell/Teacher_Add.xlsx
+++ b/file_excell/Teacher_Add.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProjectStudentSKRU_NEW\file_excell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF7E06B-7B21-484D-B89A-D34BB114079D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E64FF71-490A-49AD-B3D1-C0A58DEA7837}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{BAF349C9-1B8A-4E47-B48D-634E15233966}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>รหัสอาจารย์</t>
   </si>
   <si>
-    <t>ชื่อ นามสกุล</t>
-  </si>
-  <si>
     <t>อีเมลล์</t>
   </si>
   <si>
@@ -54,6 +51,15 @@
   </si>
   <si>
     <t>อาจารย์ประจำวิชา</t>
+  </si>
+  <si>
+    <t>นามสกุล</t>
+  </si>
+  <si>
+    <t>คำนำหน้า</t>
+  </si>
+  <si>
+    <t>ชื่อ</t>
   </si>
 </sst>
 </file>
@@ -425,76 +431,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB4135A-6F84-41C4-B33A-3A0E38EACD9A}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D12"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="E3" s="1"/>
+      <c r="I3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="C3" s="1"/>
-      <c r="G3" t="s">
+    <row r="4" spans="1:10">
+      <c r="E4" s="1"/>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="C4" s="1"/>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
+    <row r="5" spans="1:10">
+      <c r="E5" s="1"/>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="C5" s="1"/>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="C11" s="1"/>
+    <row r="6" spans="1:10">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>